<commit_message>
ajout du cv et du tableau à jour
</commit_message>
<xml_diff>
--- a/project/public/TableauDeSynthèse.xlsx
+++ b/project/public/TableauDeSynthèse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06366BEE-57F4-4DD6-909B-B3156DE9B9E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA69946D-13FF-4E05-9DE6-FFF6BC42D18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>h</t>
   </si>
   <si>
-    <t>Centre de formation :</t>
-  </si>
-  <si>
     <t>Option :</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
   </si>
   <si>
     <t>▢ SLAM</t>
-  </si>
-  <si>
-    <t>Adresse URL du portfolio :</t>
   </si>
   <si>
     <t>Compétences mises en œuvre
@@ -172,6 +166,12 @@
   </si>
   <si>
     <t xml:space="preserve"> ×</t>
+  </si>
+  <si>
+    <t>Centre de formation : Ipssi campus de Marne-La-Vallée</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio :https://matthieu77220.github.io/portfolio/</t>
   </si>
 </sst>
 </file>
@@ -705,15 +705,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -746,45 +785,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -808,19 +808,19 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>173846</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1175658</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>184594</xdr:rowOff>
+      <xdr:rowOff>108856</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>455726</xdr:colOff>
+      <xdr:colOff>478647</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>403114</xdr:rowOff>
+      <xdr:rowOff>347879</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="4" name="Encre 3">
@@ -833,13 +833,13 @@
             <xdr14:cNvContentPartPr/>
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="13116960" y="1708594"/>
-            <a:ext cx="281880" cy="218520"/>
+          <xdr14:xfrm flipH="1" flipV="1">
+            <a:off x="13237029" y="1632856"/>
+            <a:ext cx="587504" cy="239023"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="4" name="Encre 3">
@@ -897,8 +897,8 @@
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">122 1 24575,'3'1'0,"-1"0"0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,-1 1 0,2 3 0,14 14 0,15 2 0,44 21 0,23 15 0,-87-49 0,-1 1 0,-1-1 0,1 2 0,-2 0 0,1 0 0,10 15 0,-6-7 0,1 0 0,1 0 0,27 21 0,-34-32 0,0-1 0,0 0 0,1-1 0,11 5 0,-10-4 0,0-1 0,0 1 0,12 10 0,-4-1-111,-10-7-98,1 0 0,0 0 0,0-1 0,1 0 0,20 9 0,-8-8-6617</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1862.42">1 607 24575,'0'-5'0,"1"1"0,-1 0 0,1 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 1 0,1 0 0,4-6 0,5-3 0,1 0 0,18-14 0,-21 18 0,1 0 0,-2-1 0,18-19 0,-9 6 0,37-35 0,1-1 0,-36 37 0,1 1 0,0 1 0,2 2 0,30-20 0,-24 18 0,-2-2 0,34-31 0,-57 48-227,1 1-1,-1-1 1,1 0-1,0 1 1,6-3-1,7-2-6598</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1378 666 24575,'-6'-1'0,"1"0"0,1 0 0,0 0 0,0-2 0,0 2 0,0-1 0,-1 1 0,1-1 0,2 0 0,-2-1 0,0 2 0,2-1 0,-4-3 0,-30-16 0,-31-2 0,-91-23 0,-48-16 0,181 53 0,2-1 0,2 1 0,-2-2 0,4 0 0,-2 0 0,-20-16 0,11 7 0,-1 1 0,-2-1 0,-57-23 0,72 36 0,-1 0 0,0 1 0,-2 0 0,-23-5 0,21 5 0,1 0 0,-1 0 0,-25-12 0,8 2-111,21 7-98,-2 0 0,1 0 0,-1 2 0,-2-1 0,-42-9 0,17 8-6617</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1862.42">1630 3 24575,'0'6'0,"-2"-2"0,2 0 0,-2 1 0,0-1 0,0 0 0,0 0 0,-3 0 0,3 0 0,-2 1 0,0-2 0,0 1 0,0 0 0,-3-1 0,-7 7 0,-11 3 0,-2 0 0,-38 16 0,44-21 0,-2 1 0,5 1 0,-39 21 0,20-7 0,-78 38 0,-1 1 0,74-40 0,-2-1 0,0-1 0,-4-2 0,-62 21 0,49-19 0,5 2 0,-71 34 0,119-53-227,-3-1-1,3 2 1,-2-1-1,-1-1 1,-12 4-1,-14 2-6598</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1194,8 +1194,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1212,122 +1212,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="23"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="41" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="42"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="34"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="12" t="s">
+      <c r="G4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="18" t="s">
+    </row>
+    <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="47"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
+      <c r="B6" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="6" t="s">
+    </row>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="D7" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="19" t="s">
+      <c r="E7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="F7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="G7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="H7" s="20" t="s">
         <v>20</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>22</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1366,16 +1366,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
+      <c r="A8" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="39"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1414,26 +1414,26 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="44" t="s">
-        <v>36</v>
+        <v>24</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>34</v>
       </c>
       <c r="E9" s="14"/>
-      <c r="F9" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="45" t="s">
-        <v>37</v>
+      <c r="F9" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>35</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
@@ -1473,26 +1473,26 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>36</v>
+        <v>27</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="E10" s="14"/>
-      <c r="F10" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="47" t="s">
-        <v>36</v>
+      <c r="F10" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>34</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1532,26 +1532,26 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="46" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="E11" s="14"/>
-      <c r="F11" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="47" t="s">
-        <v>36</v>
+      <c r="F11" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>34</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -1591,26 +1591,26 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="46" t="s">
-        <v>36</v>
+        <v>29</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="E12" s="14"/>
-      <c r="F12" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="47" t="s">
-        <v>36</v>
+      <c r="F12" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>34</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -1919,16 +1919,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
+      <c r="A19" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="42"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1967,26 +1967,26 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="46" t="s">
-        <v>36</v>
+      <c r="D20" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="E20" s="14"/>
-      <c r="F20" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="H20" s="47" t="s">
-        <v>36</v>
+      <c r="F20" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>34</v>
       </c>
       <c r="I20"/>
       <c r="J20"/>
@@ -2295,16 +2295,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="29"/>
+      <c r="A27" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="42"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2749,11 +2749,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2761,6 +2756,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2973,15 +2973,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9afeb195-fe8e-4d53-b966-ac86e014f9d0">
@@ -2990,6 +2981,15 @@
     <TaxCatchAll xmlns="b96438d6-4088-444b-a148-08e2a0c42289" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3012,14 +3012,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{574C0259-CE3C-4D74-A0FE-24A73702E787}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EA3166D-F719-49F0-B698-E9057D9EDF6C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3028,4 +3020,12 @@
     <ds:schemaRef ds:uri="b96438d6-4088-444b-a148-08e2a0c42289"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{574C0259-CE3C-4D74-A0FE-24A73702E787}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>